<commit_message>
Finished basic Perceptron code
</commit_message>
<xml_diff>
--- a/Classes/CS 450 - Computer Networks/Excel/ClassAssignment1.xlsx
+++ b/Classes/CS 450 - Computer Networks/Excel/ClassAssignment1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Strut\Documents\School\Grad School\Classes\CS 450 - Computer Networks\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CA8C42-A058-4800-B5EA-131782917BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5EDE1F-D168-4281-B790-1BB68E5A8196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{624ACCBE-F53D-4C17-AC4D-342622306D6F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="52">
   <si>
     <t>Vaccum</t>
   </si>
@@ -299,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -332,6 +332,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,7 +650,7 @@
   <dimension ref="A2:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -830,10 +831,10 @@
       <c r="C25" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -845,9 +846,12 @@
       <c r="D26" s="5">
         <v>1460</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="3">
         <f>_xlfn.CEILING.MATH(C26/D26)</f>
         <v>735440</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -872,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9112CC60-1290-495C-B4FF-B61AAE570DF7}">
   <dimension ref="A6:J83"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="B66" sqref="B1:B1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1572,8 +1576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD052EB6-2547-473E-ABA6-153D06EFEFD0}">
   <dimension ref="A2:J118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1618,7 +1622,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="4">
+      <c r="B6" s="18">
         <f>E6/F6</f>
         <v>4.3478260869565224E-7</v>
       </c>
@@ -1636,7 +1640,7 @@
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B7" s="6">
+      <c r="B7" s="18">
         <f>B6*10^3</f>
         <v>4.3478260869565224E-4</v>
       </c>
@@ -1646,7 +1650,7 @@
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="6">
+      <c r="B8" s="18">
         <f>B7*10^3</f>
         <v>0.43478260869565222</v>
       </c>
@@ -1662,7 +1666,7 @@
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="16">
+      <c r="B11" s="18">
         <f>B6*2</f>
         <v>8.6956521739130448E-7</v>
       </c>
@@ -1671,7 +1675,7 @@
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="8">
+      <c r="B12" s="18">
         <f>B7*2</f>
         <v>8.6956521739130449E-4</v>
       </c>
@@ -1680,7 +1684,7 @@
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="3">
+      <c r="B13" s="18">
         <f>B8*2</f>
         <v>0.86956521739130443</v>
       </c>
@@ -1726,7 +1730,7 @@
         <f>150*(1024*1024*1024)</f>
         <v>161061273600</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="5">
         <v>1460</v>
       </c>
     </row>
@@ -1800,7 +1804,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
-      <c r="B34" s="13">
+      <c r="B34" s="18">
         <f>E34/F34</f>
         <v>2.6086956521739131E-7</v>
       </c>
@@ -1808,10 +1812,10 @@
         <v>8</v>
       </c>
       <c r="D34" s="1"/>
-      <c r="E34" s="10">
+      <c r="E34" s="5">
         <v>60</v>
       </c>
-      <c r="F34" s="10">
+      <c r="F34" s="5">
         <f>VLOOKUP(G34, Constants!$A$2:$B$4, 2, FALSE)</f>
         <v>229999999.99999997</v>
       </c>
@@ -1824,7 +1828,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
-      <c r="B35" s="13">
+      <c r="B35" s="18">
         <f>B34*10^3</f>
         <v>2.6086956521739134E-4</v>
       </c>
@@ -1841,7 +1845,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
-      <c r="B36" s="13">
+      <c r="B36" s="18">
         <f>B35*10^3</f>
         <v>0.26086956521739135</v>
       </c>
@@ -1898,7 +1902,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
-      <c r="B40" s="13">
+      <c r="B40" s="18">
         <f>2*E40</f>
         <v>5.2173913043478263E-7</v>
       </c>
@@ -1906,7 +1910,7 @@
         <v>8</v>
       </c>
       <c r="D40" s="1"/>
-      <c r="E40" s="13">
+      <c r="E40" s="18">
         <f>B34</f>
         <v>2.6086956521739131E-7</v>
       </c>
@@ -1918,7 +1922,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
-      <c r="B41" s="13">
+      <c r="B41" s="18">
         <f>B40*10^3</f>
         <v>5.2173913043478267E-4</v>
       </c>
@@ -1935,7 +1939,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
-      <c r="B42" s="13">
+      <c r="B42" s="18">
         <f>B41*10^3</f>
         <v>0.52173913043478271</v>
       </c>
@@ -1996,7 +2000,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
-      <c r="B46" s="15">
+      <c r="B46" s="18">
         <f>G46/E46</f>
         <v>85.899345920000002</v>
       </c>
@@ -2022,7 +2026,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
-      <c r="B47" s="14">
+      <c r="B47" s="4">
         <f>B46*10^3</f>
         <v>85899.345920000007</v>
       </c>
@@ -2039,7 +2043,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
-      <c r="B48" s="3">
+      <c r="B48" s="6">
         <f>B47*10^3</f>
         <v>85899345.920000002</v>
       </c>
@@ -2112,7 +2116,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="1"/>
-      <c r="B53" s="9">
+      <c r="B53" s="14">
         <f>E53/F53</f>
         <v>8.9999999999999993E-3</v>
       </c>
@@ -2120,11 +2124,11 @@
         <v>8</v>
       </c>
       <c r="D53" s="1"/>
-      <c r="E53" s="10">
+      <c r="E53" s="5">
         <f>1800*10^3</f>
         <v>1800000</v>
       </c>
-      <c r="F53" s="10">
+      <c r="F53" s="5">
         <f>VLOOKUP(G53, Constants!$A$2:$B$4, 2, FALSE)</f>
         <v>200000000</v>
       </c>
@@ -2211,7 +2215,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="1"/>
-      <c r="B59" s="13">
+      <c r="B59" s="14">
         <f>2*E59</f>
         <v>1.7999999999999999E-2</v>
       </c>
@@ -2219,7 +2223,7 @@
         <v>8</v>
       </c>
       <c r="D59" s="1"/>
-      <c r="E59" s="13">
+      <c r="E59" s="14">
         <f>B53</f>
         <v>8.9999999999999993E-3</v>
       </c>
@@ -2231,7 +2235,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="1"/>
-      <c r="B60" s="13">
+      <c r="B60" s="6">
         <f>B59*10^3</f>
         <v>18</v>
       </c>
@@ -2248,7 +2252,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="1"/>
-      <c r="B61" s="13">
+      <c r="B61" s="3">
         <f>B60*10^3</f>
         <v>18000</v>
       </c>
@@ -2309,7 +2313,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="1"/>
-      <c r="B65" s="16">
+      <c r="B65" s="18">
         <f>G65/E65</f>
         <v>21.47483648</v>
       </c>
@@ -2335,7 +2339,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="1"/>
-      <c r="B66" s="9">
+      <c r="B66" s="15">
         <f>B65*10^3</f>
         <v>21474.836480000002</v>
       </c>
@@ -2352,7 +2356,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="1"/>
-      <c r="B67" s="8">
+      <c r="B67" s="14">
         <f>B66*10^3</f>
         <v>21474836.48</v>
       </c>
@@ -2425,7 +2429,7 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="1"/>
-      <c r="B72" s="13">
+      <c r="B72" s="18">
         <f>E72/F72</f>
         <v>3.91304347826087E-7</v>
       </c>
@@ -2437,7 +2441,7 @@
         <f>90</f>
         <v>90</v>
       </c>
-      <c r="F72" s="10">
+      <c r="F72" s="5">
         <f>VLOOKUP(G72, Constants!$A$2:$B$4, 2, FALSE)</f>
         <v>229999999.99999997</v>
       </c>
@@ -2450,7 +2454,7 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="1"/>
-      <c r="B73" s="13">
+      <c r="B73" s="18">
         <f>B72*10^3</f>
         <v>3.9130434782608698E-4</v>
       </c>
@@ -2467,7 +2471,7 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="1"/>
-      <c r="B74" s="13">
+      <c r="B74" s="18">
         <f>B73*10^3</f>
         <v>0.39130434782608697</v>
       </c>
@@ -2524,7 +2528,7 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="1"/>
-      <c r="B78" s="13">
+      <c r="B78" s="18">
         <f>2*E78</f>
         <v>7.8260869565217399E-7</v>
       </c>
@@ -2532,7 +2536,7 @@
         <v>8</v>
       </c>
       <c r="D78" s="1"/>
-      <c r="E78" s="13">
+      <c r="E78" s="18">
         <f>B72</f>
         <v>3.91304347826087E-7</v>
       </c>
@@ -2544,7 +2548,7 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="1"/>
-      <c r="B79" s="13">
+      <c r="B79" s="18">
         <f>B78*10^3</f>
         <v>7.8260869565217395E-4</v>
       </c>
@@ -2561,7 +2565,7 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="1"/>
-      <c r="B80" s="13">
+      <c r="B80" s="18">
         <f>B79*10^3</f>
         <v>0.78260869565217395</v>
       </c>
@@ -2748,7 +2752,7 @@
         <f>F46</f>
         <v>107374182400</v>
       </c>
-      <c r="F91" s="10">
+      <c r="F91" s="5">
         <v>1460</v>
       </c>
       <c r="G91" s="1"/>
@@ -2800,7 +2804,7 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="1"/>
-      <c r="B95" s="6">
+      <c r="B95" s="15">
         <f>E95*F95</f>
         <v>2941.7584399999996</v>
       </c>
@@ -2823,7 +2827,7 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="1"/>
-      <c r="B96" s="6">
+      <c r="B96" s="14">
         <f>B95*10^3</f>
         <v>2941758.4399999995</v>
       </c>
@@ -2840,7 +2844,7 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="1"/>
-      <c r="B97" s="6">
+      <c r="B97" s="3">
         <f>B96*10^3</f>
         <v>2941758439.9999995</v>
       </c>
@@ -2905,7 +2909,7 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="1"/>
-      <c r="B101" s="13">
+      <c r="B101" s="18">
         <f>E101+(2*F101)+G101+(2*H101)+I101</f>
         <v>1.8161304347826084E-2</v>
       </c>
@@ -2954,7 +2958,7 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="1"/>
-      <c r="B103" s="6">
+      <c r="B103" s="14">
         <f>B102*10^3</f>
         <v>18161.304347826081</v>
       </c>
@@ -3029,11 +3033,11 @@
         <v>8</v>
       </c>
       <c r="D107" s="1"/>
-      <c r="E107" s="15">
+      <c r="E107" s="18">
         <f>3*B101</f>
         <v>5.4483913043478251E-2</v>
       </c>
-      <c r="F107" s="15">
+      <c r="F107" s="18">
         <f>B34+B46</f>
         <v>85.899346180869571</v>
       </c>
@@ -3041,7 +3045,7 @@
         <f>B95</f>
         <v>2941.7584399999996</v>
       </c>
-      <c r="H107" s="15">
+      <c r="H107" s="18">
         <f>B53+B65</f>
         <v>21.483836480000001</v>
       </c>
@@ -3049,7 +3053,7 @@
         <f>B95</f>
         <v>2941.7584399999996</v>
       </c>
-      <c r="J107" s="15">
+      <c r="J107" s="18">
         <f>B72+B84</f>
         <v>858.99345959130426</v>
       </c>

</xml_diff>